<commit_message>
Atualização base de obras Douglas Cezar
</commit_message>
<xml_diff>
--- a/data/obras-cadastradas-DOUGLAS-CEZAR_iswc.xlsx
+++ b/data/obras-cadastradas-DOUGLAS-CEZAR_iswc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\ROYALTY\_ANALYTICS_\Python Codes\Nas Nuvens App\nasnuvens-app\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95250FE4-3DAC-4C91-A7F7-B309165ECF17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{340B5F52-65F5-4D32-9095-6BE2D85D178A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A6FA0D54-048B-4B92-8897-C48693123731}"/>
   </bookViews>
@@ -1714,7 +1714,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{750FA41E-4BC6-485D-85BC-747E37A1B6AD}">
   <dimension ref="A1:E225"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="C46" sqref="A46:XFD46"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2491,13 +2493,13 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46">
-        <v>13613451</v>
+        <v>24088018</v>
       </c>
       <c r="B46" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="C46" t="s">
-        <v>143</v>
+        <v>22</v>
       </c>
       <c r="D46" t="s">
         <v>121</v>
@@ -2508,13 +2510,13 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47">
-        <v>24088018</v>
+        <v>15020538</v>
       </c>
       <c r="B47" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C47" t="s">
-        <v>22</v>
+        <v>144</v>
       </c>
       <c r="D47" t="s">
         <v>121</v>
@@ -2525,13 +2527,13 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48">
-        <v>15020538</v>
+        <v>8205212</v>
       </c>
       <c r="B48" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="C48" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D48" t="s">
         <v>121</v>
@@ -2542,13 +2544,13 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49">
-        <v>8205212</v>
+        <v>24287609</v>
       </c>
       <c r="B49" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="C49" t="s">
-        <v>145</v>
+        <v>23</v>
       </c>
       <c r="D49" t="s">
         <v>121</v>
@@ -2559,13 +2561,13 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50">
-        <v>24287609</v>
+        <v>16542347</v>
       </c>
       <c r="B50" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="C50" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D50" t="s">
         <v>121</v>
@@ -2576,13 +2578,13 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51">
-        <v>16542347</v>
+        <v>13375686</v>
       </c>
       <c r="B51" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="C51" t="s">
-        <v>24</v>
+        <v>146</v>
       </c>
       <c r="D51" t="s">
         <v>121</v>
@@ -2593,13 +2595,13 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52">
-        <v>13375686</v>
+        <v>29698365</v>
       </c>
       <c r="B52" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="C52" t="s">
-        <v>146</v>
+        <v>25</v>
       </c>
       <c r="D52" t="s">
         <v>121</v>
@@ -2610,13 +2612,13 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53">
-        <v>29698365</v>
+        <v>32056368</v>
       </c>
       <c r="B53" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="C53" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D53" t="s">
         <v>121</v>
@@ -2627,13 +2629,13 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54">
-        <v>32056368</v>
+        <v>25962956</v>
       </c>
       <c r="B54" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="C54" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D54" t="s">
         <v>121</v>
@@ -2644,13 +2646,13 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55">
-        <v>25962956</v>
+        <v>16161643</v>
       </c>
       <c r="B55" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C55" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D55" t="s">
         <v>121</v>
@@ -2661,13 +2663,13 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56">
-        <v>16161643</v>
+        <v>24088041</v>
       </c>
       <c r="B56" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="C56" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D56" t="s">
         <v>121</v>
@@ -2678,13 +2680,13 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57">
-        <v>24088041</v>
+        <v>25932789</v>
       </c>
       <c r="B57" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C57" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D57" t="s">
         <v>121</v>
@@ -2695,13 +2697,13 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58">
-        <v>25932789</v>
+        <v>16491386</v>
       </c>
       <c r="B58" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="C58" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D58" t="s">
         <v>121</v>
@@ -2712,13 +2714,13 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59">
-        <v>16491386</v>
+        <v>7198714</v>
       </c>
       <c r="B59" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="C59" t="s">
-        <v>31</v>
+        <v>147</v>
       </c>
       <c r="D59" t="s">
         <v>121</v>
@@ -2729,13 +2731,13 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60">
-        <v>7198714</v>
+        <v>31901370</v>
       </c>
       <c r="B60" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C60" t="s">
-        <v>147</v>
+        <v>32</v>
       </c>
       <c r="D60" t="s">
         <v>121</v>
@@ -2746,13 +2748,13 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61">
-        <v>31901370</v>
+        <v>32457191</v>
       </c>
       <c r="B61" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="C61" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D61" t="s">
         <v>121</v>
@@ -2763,13 +2765,13 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62">
-        <v>32457191</v>
+        <v>34449440</v>
       </c>
       <c r="B62" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="C62" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D62" t="s">
         <v>121</v>
@@ -2780,10 +2782,10 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63">
-        <v>34449440</v>
+        <v>36100226</v>
       </c>
       <c r="B63" t="s">
-        <v>282</v>
+        <v>434</v>
       </c>
       <c r="C63" t="s">
         <v>34</v>
@@ -2797,13 +2799,13 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64">
-        <v>36100226</v>
+        <v>16595702</v>
       </c>
       <c r="B64" t="s">
-        <v>434</v>
+        <v>283</v>
       </c>
       <c r="C64" t="s">
-        <v>34</v>
+        <v>148</v>
       </c>
       <c r="D64" t="s">
         <v>121</v>
@@ -2814,13 +2816,13 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65">
-        <v>16595702</v>
+        <v>13600678</v>
       </c>
       <c r="B65" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="C65" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D65" t="s">
         <v>121</v>
@@ -2831,13 +2833,13 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66">
-        <v>13600678</v>
+        <v>27523769</v>
       </c>
       <c r="B66" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="C66" t="s">
-        <v>149</v>
+        <v>35</v>
       </c>
       <c r="D66" t="s">
         <v>121</v>
@@ -2848,13 +2850,13 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67">
-        <v>27523769</v>
+        <v>15020543</v>
       </c>
       <c r="B67" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C67" t="s">
-        <v>35</v>
+        <v>150</v>
       </c>
       <c r="D67" t="s">
         <v>121</v>
@@ -2865,13 +2867,13 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68">
-        <v>15020543</v>
+        <v>4713272</v>
       </c>
       <c r="B68" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="C68" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D68" t="s">
         <v>121</v>
@@ -2882,13 +2884,13 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69">
-        <v>4713272</v>
+        <v>29402709</v>
       </c>
       <c r="B69" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="C69" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D69" t="s">
         <v>121</v>
@@ -2899,13 +2901,13 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70">
-        <v>29402709</v>
+        <v>4713279</v>
       </c>
       <c r="B70" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C70" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D70" t="s">
         <v>121</v>
@@ -2916,13 +2918,13 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71">
-        <v>4713279</v>
+        <v>29602765</v>
       </c>
       <c r="B71" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="C71" t="s">
-        <v>153</v>
+        <v>36</v>
       </c>
       <c r="D71" t="s">
         <v>121</v>
@@ -2933,13 +2935,13 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72">
-        <v>29602765</v>
+        <v>14645728</v>
       </c>
       <c r="B72" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="C72" t="s">
-        <v>36</v>
+        <v>154</v>
       </c>
       <c r="D72" t="s">
         <v>121</v>
@@ -2950,13 +2952,13 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73">
-        <v>14645728</v>
+        <v>28902412</v>
       </c>
       <c r="B73" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C73" t="s">
-        <v>154</v>
+        <v>37</v>
       </c>
       <c r="D73" t="s">
         <v>121</v>
@@ -2967,13 +2969,13 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74">
-        <v>28902412</v>
+        <v>16924524</v>
       </c>
       <c r="B74" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="C74" t="s">
-        <v>37</v>
+        <v>155</v>
       </c>
       <c r="D74" t="s">
         <v>121</v>
@@ -2984,13 +2986,13 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75">
-        <v>16924524</v>
+        <v>26809058</v>
       </c>
       <c r="B75" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="C75" t="s">
-        <v>155</v>
+        <v>38</v>
       </c>
       <c r="D75" t="s">
         <v>121</v>
@@ -3001,13 +3003,13 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76">
-        <v>26809058</v>
+        <v>34541889</v>
       </c>
       <c r="B76" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C76" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D76" t="s">
         <v>121</v>
@@ -3018,13 +3020,13 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77">
-        <v>34541889</v>
+        <v>30720832</v>
       </c>
       <c r="B77" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C77" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D77" t="s">
         <v>121</v>
@@ -3035,13 +3037,13 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78">
-        <v>30720832</v>
+        <v>29402708</v>
       </c>
       <c r="B78" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C78" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D78" t="s">
         <v>121</v>
@@ -3052,13 +3054,13 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79">
-        <v>29402708</v>
+        <v>8502492</v>
       </c>
       <c r="B79" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="C79" t="s">
-        <v>41</v>
+        <v>156</v>
       </c>
       <c r="D79" t="s">
         <v>121</v>
@@ -3069,13 +3071,13 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80">
-        <v>8502492</v>
+        <v>27523771</v>
       </c>
       <c r="B80" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="C80" t="s">
-        <v>156</v>
+        <v>42</v>
       </c>
       <c r="D80" t="s">
         <v>121</v>
@@ -3086,13 +3088,13 @@
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81">
-        <v>27523771</v>
+        <v>17032055</v>
       </c>
       <c r="B81" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="C81" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D81" t="s">
         <v>121</v>
@@ -3103,13 +3105,13 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82">
-        <v>17032055</v>
+        <v>6547410</v>
       </c>
       <c r="B82" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="C82" t="s">
-        <v>43</v>
+        <v>157</v>
       </c>
       <c r="D82" t="s">
         <v>121</v>
@@ -3120,13 +3122,13 @@
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83">
-        <v>6547410</v>
+        <v>32071339</v>
       </c>
       <c r="B83" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="C83" t="s">
-        <v>157</v>
+        <v>44</v>
       </c>
       <c r="D83" t="s">
         <v>121</v>
@@ -3137,13 +3139,13 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84">
-        <v>32071339</v>
+        <v>31992713</v>
       </c>
       <c r="B84" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="C84" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D84" t="s">
         <v>121</v>
@@ -3154,13 +3156,13 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85">
-        <v>31992713</v>
+        <v>31983963</v>
       </c>
       <c r="B85" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="C85" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D85" t="s">
         <v>121</v>
@@ -3171,13 +3173,13 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86">
-        <v>31983963</v>
+        <v>16480706</v>
       </c>
       <c r="B86" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="C86" t="s">
-        <v>46</v>
+        <v>158</v>
       </c>
       <c r="D86" t="s">
         <v>121</v>
@@ -3188,13 +3190,13 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87">
-        <v>16480706</v>
+        <v>31494072</v>
       </c>
       <c r="B87" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="C87" t="s">
-        <v>158</v>
+        <v>47</v>
       </c>
       <c r="D87" t="s">
         <v>121</v>
@@ -3205,13 +3207,13 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88">
-        <v>31494072</v>
+        <v>7169431</v>
       </c>
       <c r="B88" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C88" t="s">
-        <v>47</v>
+        <v>159</v>
       </c>
       <c r="D88" t="s">
         <v>121</v>
@@ -3222,13 +3224,13 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89">
-        <v>7169431</v>
+        <v>20539490</v>
       </c>
       <c r="B89" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="C89" t="s">
-        <v>159</v>
+        <v>48</v>
       </c>
       <c r="D89" t="s">
         <v>121</v>
@@ -3239,13 +3241,13 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90">
-        <v>20539490</v>
+        <v>18900242</v>
       </c>
       <c r="B90" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="C90" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D90" t="s">
         <v>121</v>
@@ -3256,13 +3258,13 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91">
-        <v>18900242</v>
+        <v>15271768</v>
       </c>
       <c r="B91" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="C91" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D91" t="s">
         <v>121</v>
@@ -3273,10 +3275,10 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92">
-        <v>15271768</v>
+        <v>39017442</v>
       </c>
       <c r="B92" t="s">
-        <v>310</v>
+        <v>434</v>
       </c>
       <c r="C92" t="s">
         <v>50</v>
@@ -3290,13 +3292,13 @@
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93">
-        <v>39017442</v>
+        <v>13375687</v>
       </c>
       <c r="B93" t="s">
-        <v>434</v>
+        <v>311</v>
       </c>
       <c r="C93" t="s">
-        <v>50</v>
+        <v>160</v>
       </c>
       <c r="D93" t="s">
         <v>121</v>
@@ -3307,13 +3309,13 @@
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94">
-        <v>13375687</v>
+        <v>6547411</v>
       </c>
       <c r="B94" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="C94" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D94" t="s">
         <v>121</v>
@@ -3324,13 +3326,13 @@
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95">
-        <v>6547411</v>
+        <v>8205217</v>
       </c>
       <c r="B95" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="C95" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D95" t="s">
         <v>121</v>
@@ -3341,13 +3343,13 @@
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96">
-        <v>8205217</v>
+        <v>30544265</v>
       </c>
       <c r="B96" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="C96" t="s">
-        <v>162</v>
+        <v>51</v>
       </c>
       <c r="D96" t="s">
         <v>121</v>
@@ -3358,16 +3360,16 @@
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97">
-        <v>30544265</v>
+        <v>38961642</v>
       </c>
       <c r="B97" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="C97" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D97" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E97" t="s">
         <v>121</v>
@@ -3375,16 +3377,16 @@
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98">
-        <v>38961642</v>
+        <v>33145175</v>
       </c>
       <c r="B98" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="C98" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D98" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E98" t="s">
         <v>121</v>
@@ -3392,13 +3394,13 @@
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99">
-        <v>33145175</v>
+        <v>17120952</v>
       </c>
       <c r="B99" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="C99" t="s">
-        <v>53</v>
+        <v>163</v>
       </c>
       <c r="D99" t="s">
         <v>121</v>
@@ -3409,13 +3411,13 @@
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100">
-        <v>17120952</v>
+        <v>23022775</v>
       </c>
       <c r="B100" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="C100" t="s">
-        <v>163</v>
+        <v>54</v>
       </c>
       <c r="D100" t="s">
         <v>121</v>
@@ -3426,13 +3428,13 @@
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101">
-        <v>23022775</v>
+        <v>17515833</v>
       </c>
       <c r="B101" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="C101" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D101" t="s">
         <v>121</v>
@@ -3443,13 +3445,13 @@
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102">
-        <v>17515833</v>
+        <v>17902059</v>
       </c>
       <c r="B102" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="C102" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D102" t="s">
         <v>121</v>
@@ -3460,10 +3462,10 @@
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103">
-        <v>17902059</v>
+        <v>31281775</v>
       </c>
       <c r="B103" t="s">
-        <v>320</v>
+        <v>434</v>
       </c>
       <c r="C103" t="s">
         <v>56</v>
@@ -3477,13 +3479,13 @@
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104">
-        <v>31281775</v>
+        <v>7879492</v>
       </c>
       <c r="B104" t="s">
-        <v>434</v>
+        <v>321</v>
       </c>
       <c r="C104" t="s">
-        <v>56</v>
+        <v>164</v>
       </c>
       <c r="D104" t="s">
         <v>121</v>
@@ -3494,13 +3496,13 @@
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105">
-        <v>7879492</v>
+        <v>27523777</v>
       </c>
       <c r="B105" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="C105" t="s">
-        <v>164</v>
+        <v>57</v>
       </c>
       <c r="D105" t="s">
         <v>121</v>
@@ -3511,13 +3513,13 @@
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106">
-        <v>27523777</v>
+        <v>5794839</v>
       </c>
       <c r="B106" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="C106" t="s">
-        <v>57</v>
+        <v>165</v>
       </c>
       <c r="D106" t="s">
         <v>121</v>
@@ -3528,13 +3530,13 @@
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107">
-        <v>5794839</v>
+        <v>26688023</v>
       </c>
       <c r="B107" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="C107" t="s">
-        <v>165</v>
+        <v>58</v>
       </c>
       <c r="D107" t="s">
         <v>121</v>
@@ -3545,13 +3547,13 @@
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108">
-        <v>26688023</v>
+        <v>5794842</v>
       </c>
       <c r="B108" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C108" t="s">
-        <v>58</v>
+        <v>166</v>
       </c>
       <c r="D108" t="s">
         <v>121</v>
@@ -3562,13 +3564,13 @@
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109">
-        <v>5794842</v>
+        <v>6547412</v>
       </c>
       <c r="B109" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="C109" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D109" t="s">
         <v>121</v>
@@ -3579,13 +3581,13 @@
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A110">
-        <v>6547412</v>
+        <v>11658532</v>
       </c>
       <c r="B110" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="C110" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D110" t="s">
         <v>121</v>
@@ -3596,13 +3598,13 @@
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A111">
-        <v>11658532</v>
+        <v>21946482</v>
       </c>
       <c r="B111" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="C111" t="s">
-        <v>168</v>
+        <v>59</v>
       </c>
       <c r="D111" t="s">
         <v>121</v>
@@ -3613,13 +3615,13 @@
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A112">
-        <v>21946482</v>
+        <v>8502495</v>
       </c>
       <c r="B112" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="C112" t="s">
-        <v>59</v>
+        <v>169</v>
       </c>
       <c r="D112" t="s">
         <v>121</v>
@@ -3630,16 +3632,16 @@
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A113">
-        <v>8502495</v>
+        <v>37328532</v>
       </c>
       <c r="B113" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="C113" t="s">
-        <v>169</v>
+        <v>60</v>
       </c>
       <c r="D113" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E113" t="s">
         <v>121</v>
@@ -3647,10 +3649,10 @@
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A114">
-        <v>37328532</v>
+        <v>38898201</v>
       </c>
       <c r="B114" t="s">
-        <v>330</v>
+        <v>434</v>
       </c>
       <c r="C114" t="s">
         <v>60</v>
@@ -3664,16 +3666,16 @@
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A115">
-        <v>38898201</v>
+        <v>34418141</v>
       </c>
       <c r="B115" t="s">
-        <v>434</v>
+        <v>331</v>
       </c>
       <c r="C115" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D115" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E115" t="s">
         <v>121</v>
@@ -3681,13 +3683,13 @@
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A116">
-        <v>34418141</v>
+        <v>31760280</v>
       </c>
       <c r="B116" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="C116" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D116" t="s">
         <v>121</v>
@@ -3698,13 +3700,13 @@
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A117">
-        <v>31760280</v>
+        <v>6547413</v>
       </c>
       <c r="B117" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="C117" t="s">
-        <v>62</v>
+        <v>170</v>
       </c>
       <c r="D117" t="s">
         <v>121</v>
@@ -3715,13 +3717,13 @@
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A118">
-        <v>6547413</v>
+        <v>13375688</v>
       </c>
       <c r="B118" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="C118" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D118" t="s">
         <v>121</v>
@@ -3732,13 +3734,13 @@
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A119">
-        <v>13375688</v>
+        <v>14581999</v>
       </c>
       <c r="B119" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="C119" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D119" t="s">
         <v>121</v>
@@ -3749,13 +3751,13 @@
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A120">
-        <v>14581999</v>
+        <v>13375691</v>
       </c>
       <c r="B120" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="C120" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D120" t="s">
         <v>121</v>
@@ -3766,13 +3768,13 @@
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A121">
-        <v>13375691</v>
+        <v>30720830</v>
       </c>
       <c r="B121" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="C121" t="s">
-        <v>173</v>
+        <v>63</v>
       </c>
       <c r="D121" t="s">
         <v>121</v>
@@ -3783,13 +3785,13 @@
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122">
-        <v>30720830</v>
+        <v>7786979</v>
       </c>
       <c r="B122" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="C122" t="s">
-        <v>63</v>
+        <v>174</v>
       </c>
       <c r="D122" t="s">
         <v>121</v>
@@ -3800,13 +3802,13 @@
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A123">
-        <v>7786979</v>
+        <v>7807348</v>
       </c>
       <c r="B123" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="C123" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D123" t="s">
         <v>121</v>
@@ -3817,16 +3819,16 @@
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A124">
-        <v>7807348</v>
+        <v>38233255</v>
       </c>
       <c r="B124" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="C124" t="s">
-        <v>175</v>
+        <v>64</v>
       </c>
       <c r="D124" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E124" t="s">
         <v>121</v>
@@ -3834,16 +3836,16 @@
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A125">
-        <v>38233255</v>
+        <v>13113718</v>
       </c>
       <c r="B125" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="C125" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D125" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E125" t="s">
         <v>121</v>
@@ -3851,13 +3853,13 @@
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A126">
-        <v>13113718</v>
+        <v>6547414</v>
       </c>
       <c r="B126" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="C126" t="s">
-        <v>65</v>
+        <v>176</v>
       </c>
       <c r="D126" t="s">
         <v>121</v>
@@ -3868,13 +3870,13 @@
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A127">
-        <v>6547414</v>
+        <v>13113721</v>
       </c>
       <c r="B127" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="C127" t="s">
-        <v>176</v>
+        <v>66</v>
       </c>
       <c r="D127" t="s">
         <v>121</v>
@@ -3885,13 +3887,13 @@
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A128">
-        <v>13113721</v>
+        <v>31488948</v>
       </c>
       <c r="B128" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="C128" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D128" t="s">
         <v>121</v>
@@ -3902,13 +3904,13 @@
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A129">
-        <v>31488948</v>
+        <v>7879235</v>
       </c>
       <c r="B129" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="C129" t="s">
-        <v>67</v>
+        <v>177</v>
       </c>
       <c r="D129" t="s">
         <v>121</v>
@@ -3919,13 +3921,13 @@
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A130">
-        <v>7879235</v>
+        <v>7655107</v>
       </c>
       <c r="B130" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="C130" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D130" t="s">
         <v>121</v>
@@ -3936,13 +3938,13 @@
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A131">
-        <v>7655107</v>
+        <v>13504717</v>
       </c>
       <c r="B131" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="C131" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D131" t="s">
         <v>121</v>
@@ -3953,16 +3955,16 @@
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A132">
-        <v>13504717</v>
+        <v>40446256</v>
       </c>
       <c r="B132" t="s">
-        <v>347</v>
+        <v>434</v>
       </c>
       <c r="C132" t="s">
-        <v>179</v>
+        <v>68</v>
       </c>
       <c r="D132" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E132" t="s">
         <v>121</v>
@@ -3970,7 +3972,7 @@
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A133">
-        <v>40446256</v>
+        <v>40542658</v>
       </c>
       <c r="B133" t="s">
         <v>434</v>
@@ -3987,16 +3989,16 @@
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A134">
-        <v>40542658</v>
+        <v>16767354</v>
       </c>
       <c r="B134" t="s">
-        <v>434</v>
+        <v>348</v>
       </c>
       <c r="C134" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D134" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E134" t="s">
         <v>121</v>
@@ -4004,13 +4006,13 @@
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A135">
-        <v>16767354</v>
+        <v>17336528</v>
       </c>
       <c r="B135" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="C135" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D135" t="s">
         <v>121</v>
@@ -4021,13 +4023,13 @@
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A136">
-        <v>17336528</v>
+        <v>12521273</v>
       </c>
       <c r="B136" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="C136" t="s">
-        <v>70</v>
+        <v>180</v>
       </c>
       <c r="D136" t="s">
         <v>121</v>
@@ -4038,16 +4040,16 @@
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A137">
-        <v>12521273</v>
+        <v>40143698</v>
       </c>
       <c r="B137" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="C137" t="s">
-        <v>180</v>
+        <v>71</v>
       </c>
       <c r="D137" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E137" t="s">
         <v>121</v>
@@ -4055,16 +4057,16 @@
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A138">
-        <v>40143698</v>
+        <v>16793097</v>
       </c>
       <c r="B138" t="s">
-        <v>351</v>
+        <v>434</v>
       </c>
       <c r="C138" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D138" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E138" t="s">
         <v>121</v>
@@ -4072,13 +4074,13 @@
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A139">
-        <v>16793097</v>
+        <v>14861147</v>
       </c>
       <c r="B139" t="s">
-        <v>434</v>
+        <v>352</v>
       </c>
       <c r="C139" t="s">
-        <v>72</v>
+        <v>181</v>
       </c>
       <c r="D139" t="s">
         <v>121</v>
@@ -4089,13 +4091,13 @@
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A140">
-        <v>14861147</v>
+        <v>5794846</v>
       </c>
       <c r="B140" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C140" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="D140" t="s">
         <v>121</v>
@@ -4106,13 +4108,13 @@
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A141">
-        <v>5794846</v>
+        <v>29716950</v>
       </c>
       <c r="B141" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="C141" t="s">
-        <v>182</v>
+        <v>73</v>
       </c>
       <c r="D141" t="s">
         <v>121</v>
@@ -4123,13 +4125,13 @@
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A142">
-        <v>29716950</v>
+        <v>24063238</v>
       </c>
       <c r="B142" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="C142" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D142" t="s">
         <v>121</v>
@@ -4140,13 +4142,13 @@
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A143">
-        <v>24063238</v>
+        <v>25934138</v>
       </c>
       <c r="B143" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="C143" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D143" t="s">
         <v>121</v>
@@ -4157,13 +4159,13 @@
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A144">
-        <v>25934138</v>
+        <v>8205307</v>
       </c>
       <c r="B144" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="C144" t="s">
-        <v>75</v>
+        <v>183</v>
       </c>
       <c r="D144" t="s">
         <v>121</v>
@@ -4174,16 +4176,16 @@
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A145">
-        <v>8205307</v>
+        <v>36213181</v>
       </c>
       <c r="B145" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="C145" t="s">
-        <v>183</v>
+        <v>76</v>
       </c>
       <c r="D145" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E145" t="s">
         <v>121</v>
@@ -4191,16 +4193,16 @@
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A146">
-        <v>36213181</v>
+        <v>14645730</v>
       </c>
       <c r="B146" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="C146" t="s">
-        <v>76</v>
+        <v>184</v>
       </c>
       <c r="D146" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E146" t="s">
         <v>121</v>
@@ -4208,13 +4210,13 @@
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A147">
-        <v>14645730</v>
+        <v>12521274</v>
       </c>
       <c r="B147" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="C147" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D147" t="s">
         <v>121</v>
@@ -4225,13 +4227,13 @@
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A148">
-        <v>12521274</v>
+        <v>13411029</v>
       </c>
       <c r="B148" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="C148" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D148" t="s">
         <v>121</v>
@@ -4242,13 +4244,13 @@
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A149">
-        <v>13411029</v>
+        <v>7807352</v>
       </c>
       <c r="B149" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="C149" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D149" t="s">
         <v>121</v>
@@ -4259,13 +4261,13 @@
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A150">
-        <v>7807352</v>
+        <v>13134911</v>
       </c>
       <c r="B150" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="C150" t="s">
-        <v>187</v>
+        <v>77</v>
       </c>
       <c r="D150" t="s">
         <v>121</v>
@@ -4276,13 +4278,13 @@
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A151">
-        <v>13134911</v>
+        <v>27480596</v>
       </c>
       <c r="B151" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="C151" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D151" t="s">
         <v>121</v>
@@ -4293,13 +4295,13 @@
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A152">
-        <v>27480596</v>
+        <v>15089066</v>
       </c>
       <c r="B152" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="C152" t="s">
-        <v>78</v>
+        <v>188</v>
       </c>
       <c r="D152" t="s">
         <v>121</v>
@@ -4310,13 +4312,13 @@
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A153">
-        <v>15089066</v>
+        <v>27480597</v>
       </c>
       <c r="B153" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="C153" t="s">
-        <v>188</v>
+        <v>79</v>
       </c>
       <c r="D153" t="s">
         <v>121</v>
@@ -4327,13 +4329,13 @@
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A154">
-        <v>27480597</v>
+        <v>5794847</v>
       </c>
       <c r="B154" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="C154" t="s">
-        <v>79</v>
+        <v>189</v>
       </c>
       <c r="D154" t="s">
         <v>121</v>
@@ -4344,13 +4346,13 @@
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A155">
-        <v>5794847</v>
+        <v>12734380</v>
       </c>
       <c r="B155" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="C155" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="D155" t="s">
         <v>121</v>
@@ -4361,13 +4363,13 @@
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A156">
-        <v>12734380</v>
+        <v>7879493</v>
       </c>
       <c r="B156" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="C156" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D156" t="s">
         <v>121</v>
@@ -4378,13 +4380,13 @@
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A157">
-        <v>7879493</v>
+        <v>7807531</v>
       </c>
       <c r="B157" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="C157" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D157" t="s">
         <v>121</v>
@@ -4395,13 +4397,13 @@
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A158">
-        <v>7807531</v>
+        <v>17076934</v>
       </c>
       <c r="B158" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="C158" t="s">
-        <v>192</v>
+        <v>80</v>
       </c>
       <c r="D158" t="s">
         <v>121</v>
@@ -4412,13 +4414,13 @@
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A159">
-        <v>17076934</v>
+        <v>18951404</v>
       </c>
       <c r="B159" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="C159" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D159" t="s">
         <v>121</v>
@@ -4429,16 +4431,16 @@
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A160">
-        <v>18951404</v>
+        <v>35234833</v>
       </c>
       <c r="B160" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="C160" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D160" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E160" t="s">
         <v>121</v>
@@ -4446,16 +4448,16 @@
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A161">
-        <v>35234833</v>
+        <v>16561950</v>
       </c>
       <c r="B161" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="C161" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D161" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E161" t="s">
         <v>121</v>
@@ -4463,13 +4465,13 @@
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A162">
-        <v>16561950</v>
+        <v>5793007</v>
       </c>
       <c r="B162" t="s">
-        <v>374</v>
+        <v>434</v>
       </c>
       <c r="C162" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D162" t="s">
         <v>121</v>
@@ -4480,13 +4482,13 @@
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A163">
-        <v>5793007</v>
+        <v>23016404</v>
       </c>
       <c r="B163" t="s">
-        <v>434</v>
+        <v>375</v>
       </c>
       <c r="C163" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D163" t="s">
         <v>121</v>
@@ -4497,13 +4499,13 @@
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A164">
-        <v>23016404</v>
+        <v>11984396</v>
       </c>
       <c r="B164" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="C164" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D164" t="s">
         <v>121</v>
@@ -4514,10 +4516,10 @@
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A165">
-        <v>11984396</v>
+        <v>18900247</v>
       </c>
       <c r="B165" t="s">
-        <v>376</v>
+        <v>434</v>
       </c>
       <c r="C165" t="s">
         <v>86</v>
@@ -4531,13 +4533,13 @@
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A166">
-        <v>18900247</v>
+        <v>11259159</v>
       </c>
       <c r="B166" t="s">
-        <v>434</v>
+        <v>377</v>
       </c>
       <c r="C166" t="s">
-        <v>86</v>
+        <v>193</v>
       </c>
       <c r="D166" t="s">
         <v>121</v>
@@ -4548,13 +4550,13 @@
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A167">
-        <v>11259159</v>
+        <v>29421195</v>
       </c>
       <c r="B167" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="C167" t="s">
-        <v>193</v>
+        <v>87</v>
       </c>
       <c r="D167" t="s">
         <v>121</v>
@@ -4565,13 +4567,13 @@
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A168">
-        <v>29421195</v>
+        <v>18951405</v>
       </c>
       <c r="B168" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="C168" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D168" t="s">
         <v>121</v>
@@ -4582,16 +4584,16 @@
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A169">
-        <v>18951405</v>
+        <v>37262260</v>
       </c>
       <c r="B169" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="C169" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D169" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E169" t="s">
         <v>121</v>
@@ -4599,16 +4601,16 @@
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A170">
-        <v>37262260</v>
+        <v>7879494</v>
       </c>
       <c r="B170" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="C170" t="s">
-        <v>89</v>
+        <v>194</v>
       </c>
       <c r="D170" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E170" t="s">
         <v>121</v>
@@ -4616,13 +4618,13 @@
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A171">
-        <v>7879494</v>
+        <v>12521276</v>
       </c>
       <c r="B171" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="C171" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D171" t="s">
         <v>121</v>
@@ -4633,13 +4635,13 @@
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A172">
-        <v>12521276</v>
+        <v>16161646</v>
       </c>
       <c r="B172" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="C172" t="s">
-        <v>195</v>
+        <v>90</v>
       </c>
       <c r="D172" t="s">
         <v>121</v>
@@ -4650,13 +4652,13 @@
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A173">
-        <v>16161646</v>
+        <v>7879236</v>
       </c>
       <c r="B173" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="C173" t="s">
-        <v>90</v>
+        <v>196</v>
       </c>
       <c r="D173" t="s">
         <v>121</v>
@@ -4667,13 +4669,13 @@
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A174">
-        <v>7879236</v>
+        <v>26749000</v>
       </c>
       <c r="B174" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="C174" t="s">
-        <v>196</v>
+        <v>91</v>
       </c>
       <c r="D174" t="s">
         <v>121</v>
@@ -4684,13 +4686,13 @@
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A175">
-        <v>26749000</v>
+        <v>6547415</v>
       </c>
       <c r="B175" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="C175" t="s">
-        <v>91</v>
+        <v>197</v>
       </c>
       <c r="D175" t="s">
         <v>121</v>
@@ -4701,13 +4703,13 @@
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A176">
-        <v>6547415</v>
+        <v>14581994</v>
       </c>
       <c r="B176" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="C176" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="D176" t="s">
         <v>121</v>
@@ -4718,13 +4720,13 @@
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A177">
-        <v>14581994</v>
+        <v>25525273</v>
       </c>
       <c r="B177" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="C177" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D177" t="s">
         <v>121</v>
@@ -4735,13 +4737,13 @@
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A178">
-        <v>25525273</v>
+        <v>24063239</v>
       </c>
       <c r="B178" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="C178" t="s">
-        <v>199</v>
+        <v>92</v>
       </c>
       <c r="D178" t="s">
         <v>121</v>
@@ -4752,13 +4754,13 @@
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A179">
-        <v>24063239</v>
+        <v>7807351</v>
       </c>
       <c r="B179" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="C179" t="s">
-        <v>92</v>
+        <v>200</v>
       </c>
       <c r="D179" t="s">
         <v>121</v>
@@ -4769,13 +4771,13 @@
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A180">
-        <v>7807351</v>
+        <v>26696094</v>
       </c>
       <c r="B180" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="C180" t="s">
-        <v>200</v>
+        <v>93</v>
       </c>
       <c r="D180" t="s">
         <v>121</v>
@@ -4786,13 +4788,13 @@
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A181">
-        <v>26696094</v>
+        <v>13600763</v>
       </c>
       <c r="B181" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="C181" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D181" t="s">
         <v>121</v>
@@ -4803,13 +4805,13 @@
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A182">
-        <v>13600763</v>
+        <v>14645731</v>
       </c>
       <c r="B182" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="C182" t="s">
-        <v>94</v>
+        <v>201</v>
       </c>
       <c r="D182" t="s">
         <v>121</v>
@@ -4820,13 +4822,13 @@
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A183">
-        <v>14645731</v>
+        <v>7807533</v>
       </c>
       <c r="B183" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="C183" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="D183" t="s">
         <v>121</v>
@@ -4837,13 +4839,13 @@
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A184">
-        <v>7807533</v>
+        <v>19216757</v>
       </c>
       <c r="B184" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="C184" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="D184" t="s">
         <v>121</v>
@@ -4854,13 +4856,13 @@
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A185">
-        <v>19216757</v>
+        <v>18900263</v>
       </c>
       <c r="B185" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="C185" t="s">
-        <v>203</v>
+        <v>95</v>
       </c>
       <c r="D185" t="s">
         <v>121</v>
@@ -4871,13 +4873,13 @@
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A186">
-        <v>18900263</v>
+        <v>7807158</v>
       </c>
       <c r="B186" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="C186" t="s">
-        <v>95</v>
+        <v>204</v>
       </c>
       <c r="D186" t="s">
         <v>121</v>
@@ -4888,13 +4890,13 @@
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A187">
-        <v>7807158</v>
+        <v>30764708</v>
       </c>
       <c r="B187" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="C187" t="s">
-        <v>204</v>
+        <v>96</v>
       </c>
       <c r="D187" t="s">
         <v>121</v>
@@ -4905,16 +4907,16 @@
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A188">
-        <v>30764708</v>
+        <v>34340227</v>
       </c>
       <c r="B188" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="C188" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D188" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E188" t="s">
         <v>121</v>
@@ -4922,16 +4924,16 @@
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A189">
-        <v>34340227</v>
+        <v>7807535</v>
       </c>
       <c r="B189" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C189" t="s">
-        <v>97</v>
+        <v>205</v>
       </c>
       <c r="D189" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E189" t="s">
         <v>121</v>
@@ -4939,13 +4941,13 @@
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A190">
-        <v>7807535</v>
+        <v>10022402</v>
       </c>
       <c r="B190" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="C190" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D190" t="s">
         <v>121</v>
@@ -4956,13 +4958,13 @@
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A191">
-        <v>10022402</v>
+        <v>15020554</v>
       </c>
       <c r="B191" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="C191" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D191" t="s">
         <v>121</v>
@@ -4973,13 +4975,13 @@
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A192">
-        <v>15020554</v>
+        <v>24063240</v>
       </c>
       <c r="B192" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C192" t="s">
-        <v>207</v>
+        <v>98</v>
       </c>
       <c r="D192" t="s">
         <v>121</v>
@@ -4990,13 +4992,13 @@
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A193">
-        <v>24063240</v>
+        <v>11050335</v>
       </c>
       <c r="B193" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C193" t="s">
-        <v>98</v>
+        <v>208</v>
       </c>
       <c r="D193" t="s">
         <v>121</v>
@@ -5007,13 +5009,13 @@
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A194">
-        <v>11050335</v>
+        <v>30453428</v>
       </c>
       <c r="B194" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="C194" t="s">
-        <v>208</v>
+        <v>99</v>
       </c>
       <c r="D194" t="s">
         <v>121</v>
@@ -5024,13 +5026,13 @@
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A195">
-        <v>30453428</v>
+        <v>11259169</v>
       </c>
       <c r="B195" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="C195" t="s">
-        <v>99</v>
+        <v>209</v>
       </c>
       <c r="D195" t="s">
         <v>121</v>
@@ -5041,13 +5043,13 @@
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A196">
-        <v>11259169</v>
+        <v>7772875</v>
       </c>
       <c r="B196" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="C196" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D196" t="s">
         <v>121</v>
@@ -5058,13 +5060,13 @@
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A197">
-        <v>7772875</v>
+        <v>15858838</v>
       </c>
       <c r="B197" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="C197" t="s">
-        <v>210</v>
+        <v>100</v>
       </c>
       <c r="D197" t="s">
         <v>121</v>
@@ -5075,13 +5077,13 @@
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A198">
-        <v>15858838</v>
+        <v>24857051</v>
       </c>
       <c r="B198" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="C198" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D198" t="s">
         <v>121</v>
@@ -5092,16 +5094,16 @@
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A199">
-        <v>24857051</v>
+        <v>35051533</v>
       </c>
       <c r="B199" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="C199" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D199" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E199" t="s">
         <v>121</v>
@@ -5109,16 +5111,16 @@
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A200">
-        <v>35051533</v>
+        <v>25632409</v>
       </c>
       <c r="B200" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="C200" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D200" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E200" t="s">
         <v>121</v>
@@ -5126,13 +5128,13 @@
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A201">
-        <v>25632409</v>
+        <v>29100793</v>
       </c>
       <c r="B201" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="C201" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D201" t="s">
         <v>121</v>
@@ -5143,13 +5145,13 @@
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A202">
-        <v>29100793</v>
+        <v>12521237</v>
       </c>
       <c r="B202" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="C202" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D202" t="s">
         <v>121</v>
@@ -5160,13 +5162,13 @@
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A203">
-        <v>12521237</v>
+        <v>17120957</v>
       </c>
       <c r="B203" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="C203" t="s">
-        <v>105</v>
+        <v>211</v>
       </c>
       <c r="D203" t="s">
         <v>121</v>
@@ -5177,13 +5179,13 @@
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A204">
-        <v>17120957</v>
+        <v>13600782</v>
       </c>
       <c r="B204" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="C204" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="D204" t="s">
         <v>121</v>
@@ -5194,13 +5196,13 @@
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A205">
-        <v>13600782</v>
+        <v>34861531</v>
       </c>
       <c r="B205" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="C205" t="s">
-        <v>212</v>
+        <v>106</v>
       </c>
       <c r="D205" t="s">
         <v>121</v>
@@ -5211,13 +5213,13 @@
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A206">
-        <v>34861531</v>
+        <v>14645732</v>
       </c>
       <c r="B206" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="C206" t="s">
-        <v>106</v>
+        <v>213</v>
       </c>
       <c r="D206" t="s">
         <v>121</v>
@@ -5228,13 +5230,13 @@
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A207">
-        <v>14645732</v>
+        <v>8205227</v>
       </c>
       <c r="B207" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="C207" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D207" t="s">
         <v>121</v>
@@ -5245,13 +5247,13 @@
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A208">
-        <v>8205227</v>
+        <v>7807153</v>
       </c>
       <c r="B208" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="C208" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="D208" t="s">
         <v>121</v>
@@ -5262,13 +5264,13 @@
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A209">
-        <v>7807153</v>
+        <v>18951403</v>
       </c>
       <c r="B209" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="C209" t="s">
-        <v>215</v>
+        <v>107</v>
       </c>
       <c r="D209" t="s">
         <v>121</v>
@@ -5279,13 +5281,13 @@
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A210">
-        <v>18951403</v>
+        <v>35186450</v>
       </c>
       <c r="B210" t="s">
-        <v>420</v>
+        <v>434</v>
       </c>
       <c r="C210" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D210" t="s">
         <v>121</v>
@@ -5296,13 +5298,13 @@
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A211">
-        <v>35186450</v>
+        <v>31780026</v>
       </c>
       <c r="B211" t="s">
-        <v>434</v>
+        <v>421</v>
       </c>
       <c r="C211" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D211" t="s">
         <v>121</v>
@@ -5313,13 +5315,13 @@
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A212">
-        <v>31780026</v>
+        <v>19575257</v>
       </c>
       <c r="B212" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="C212" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D212" t="s">
         <v>121</v>
@@ -5330,13 +5332,13 @@
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A213">
-        <v>19575257</v>
+        <v>18900264</v>
       </c>
       <c r="B213" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="C213" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D213" t="s">
         <v>121</v>
@@ -5347,13 +5349,13 @@
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A214">
-        <v>18900264</v>
+        <v>13142886</v>
       </c>
       <c r="B214" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="C214" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D214" t="s">
         <v>121</v>
@@ -5364,13 +5366,13 @@
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A215">
-        <v>13142886</v>
+        <v>17456902</v>
       </c>
       <c r="B215" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="C215" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D215" t="s">
         <v>121</v>
@@ -5381,13 +5383,13 @@
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A216">
-        <v>17456902</v>
+        <v>29602767</v>
       </c>
       <c r="B216" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="C216" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D216" t="s">
         <v>121</v>
@@ -5398,13 +5400,13 @@
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A217">
-        <v>29602767</v>
+        <v>19151559</v>
       </c>
       <c r="B217" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="C217" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D217" t="s">
         <v>121</v>
@@ -5415,13 +5417,13 @@
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A218">
-        <v>19151559</v>
+        <v>7807539</v>
       </c>
       <c r="B218" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="C218" t="s">
-        <v>115</v>
+        <v>216</v>
       </c>
       <c r="D218" t="s">
         <v>121</v>
@@ -5432,13 +5434,13 @@
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A219">
-        <v>7807539</v>
+        <v>15020547</v>
       </c>
       <c r="B219" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="C219" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D219" t="s">
         <v>121</v>
@@ -5449,13 +5451,13 @@
     </row>
     <row r="220" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A220">
-        <v>15020547</v>
+        <v>25631974</v>
       </c>
       <c r="B220" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="C220" t="s">
-        <v>217</v>
+        <v>116</v>
       </c>
       <c r="D220" t="s">
         <v>121</v>
@@ -5466,13 +5468,13 @@
     </row>
     <row r="221" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A221">
-        <v>25631974</v>
+        <v>16161648</v>
       </c>
       <c r="B221" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="C221" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D221" t="s">
         <v>121</v>
@@ -5483,13 +5485,13 @@
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A222">
-        <v>16161648</v>
+        <v>11259173</v>
       </c>
       <c r="B222" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="C222" t="s">
-        <v>117</v>
+        <v>218</v>
       </c>
       <c r="D222" t="s">
         <v>121</v>
@@ -5500,13 +5502,13 @@
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A223">
-        <v>11259173</v>
+        <v>21327169</v>
       </c>
       <c r="B223" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="C223" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="D223" t="s">
         <v>121</v>
@@ -5517,16 +5519,16 @@
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A224">
-        <v>21327169</v>
+        <v>41272008</v>
       </c>
       <c r="B224" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="C224" t="s">
-        <v>219</v>
+        <v>68</v>
       </c>
       <c r="D224" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E224" t="s">
         <v>121</v>
@@ -5534,16 +5536,16 @@
     </row>
     <row r="225" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A225">
-        <v>41272008</v>
+        <v>41590407</v>
       </c>
       <c r="B225" t="s">
-        <v>434</v>
+        <v>265</v>
       </c>
       <c r="C225" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="D225" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E225" t="s">
         <v>121</v>

</xml_diff>